<commit_message>
repository to submit the code to PNAS
</commit_message>
<xml_diff>
--- a/NWH_model_results.xlsx
+++ b/NWH_model_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\.shortcut-targets-by-id\16gImdizyWRB8LaQN0Qpnrcf0CEehfkRM\Water Group\National Water Quality Paper\Submission\PNAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CA3E6D-09FF-4F71-A48A-62804284551E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{852B4AF8-F88B-41C5-A701-4F83FBDB4EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="5895" windowWidth="29040" windowHeight="15840" xr2:uid="{2D50DD0D-471F-4BC8-A6F9-10E5AFDDCCB0}"/>
   </bookViews>
@@ -1185,13 +1185,13 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Filter out lakes that are not in National Lake Assessment</t>
-  </si>
-  <si>
     <t>Distance from river</t>
   </si>
   <si>
     <t>baseline</t>
+  </si>
+  <si>
+    <t>Filter out lakes that are not in National Lake Assessment (NLA 2012)</t>
   </si>
 </sst>
 </file>
@@ -1727,8 +1727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A59FDCF8-B759-45EE-8C5C-2A04E9FA7CF0}">
   <dimension ref="A1:AM43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A9"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1739,7 +1739,7 @@
     <row r="1" spans="1:39" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="20"/>
       <c r="B1" s="23" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -6058,7 +6058,7 @@
     </row>
     <row r="39" spans="1:39" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B39" s="33" t="s">
         <v>361</v>
@@ -6264,7 +6264,7 @@
         <v>370</v>
       </c>
       <c r="AD40" s="9" t="s">
-        <v>367</v>
+        <v>353</v>
       </c>
       <c r="AE40" s="9" t="s">
         <v>367</v>
@@ -6410,7 +6410,7 @@
         <v>372</v>
       </c>
       <c r="AM41" s="8" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="42" spans="1:39" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -6532,9 +6532,9 @@
         <v>381</v>
       </c>
     </row>
-    <row r="43" spans="1:39" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:39" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="10" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="B43" s="34" t="s">
         <v>381</v>

</xml_diff>